<commit_message>
Changed the launch intent button to be Record Location
</commit_message>
<xml_diff>
--- a/app/tables/geotagger/forms/geotagger/geotagger.xlsx
+++ b/app/tables/geotagger/forms/geotagger/geotagger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5440" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Capture the GPS coordinates of this location</t>
+  </si>
+  <si>
+    <t>buttonLabel</t>
+  </si>
+  <si>
+    <t>Record Location</t>
   </si>
 </sst>
 </file>
@@ -651,23 +657,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.5" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="11" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="41.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="5"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -683,8 +690,11 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
@@ -701,7 +711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -718,7 +728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -732,7 +742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -744,6 +754,9 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -762,11 +775,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
@@ -774,7 +787,7 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -785,7 +798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -793,7 +806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -801,7 +814,7 @@
         <v>20140514</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -809,7 +822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Agriculture and selects_demo with Gruntfile.js changes for BMGF demo in October
</commit_message>
<xml_diff>
--- a/app/tables/geotagger/forms/geotagger/geotagger.xlsx
+++ b/app/tables/geotagger/forms/geotagger/geotagger.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -110,13 +110,16 @@
   </si>
   <si>
     <t>Record Location</t>
+  </si>
+  <si>
+    <t>disableSwipeNavigation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +148,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -254,7 +268,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -287,6 +301,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -773,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -830,6 +850,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>